<commit_message>
able to fin path of keys to be actived given a switch network
</commit_message>
<xml_diff>
--- a/RelayTable/RelayTable.xlsx
+++ b/RelayTable/RelayTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikocong/RelayTable/RelayTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7465E5B-D03F-2948-A6B8-845565E64CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C05241A-DEE2-C240-A9B0-75D6E89AE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2280" yWindow="460" windowWidth="14540" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,7 +627,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -755,39 +755,39 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>12</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -801,16 +801,16 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
         <v>18</v>
@@ -824,16 +824,16 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s">
         <v>18</v>
@@ -847,7 +847,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -870,7 +870,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -882,7 +882,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -893,163 +893,163 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>33</v>
+      <c r="D16" t="s">
+        <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F16" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>33</v>
+      <c r="G16" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
+      <c r="D17" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
         <v>11</v>
       </c>
-      <c r="G17" t="s">
-        <v>12</v>
+      <c r="G17" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no action on float
</commit_message>
<xml_diff>
--- a/RelayTable/RelayTable.xlsx
+++ b/RelayTable/RelayTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mikocong/RelayTable/RelayTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C05241A-DEE2-C240-A9B0-75D6E89AE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E23149D-4974-E845-96E7-D271D029B7FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="460" windowWidth="14540" windowHeight="9080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7460" yWindow="1600" windowWidth="14600" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -311,7 +311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -322,6 +322,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -626,20 +630,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -663,30 +667,30 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="5" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -708,8 +712,8 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>14</v>
+      <c r="A4" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -731,8 +735,8 @@
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>15</v>
+      <c r="A5" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -755,25 +759,25 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>66</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:7">

</xml_diff>

<commit_message>
able to write relay pin connction back to excel
</commit_message>
<xml_diff>
--- a/RelayTable/RelayTable.xlsx
+++ b/RelayTable/RelayTable.xlsx
@@ -1261,317 +1261,491 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
-        <is>
-          <t>Net_A</t>
-        </is>
-      </c>
-      <c r="B1" s="3" t="inlineStr">
-        <is>
-          <t>Net_B</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="inlineStr">
-        <is>
-          <t>Relay</t>
+      <c r="A1" s="6" t="inlineStr">
+        <is>
+          <t>Relays</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>I</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
+        <is>
+          <t>CO</t>
+        </is>
+      </c>
+      <c r="D1" s="6" t="inlineStr">
+        <is>
+          <t>CC</t>
+        </is>
+      </c>
+      <c r="E1" s="6" t="inlineStr">
+        <is>
+          <t>controlA</t>
+        </is>
+      </c>
+      <c r="F1" s="6" t="inlineStr">
+        <is>
+          <t>controlB</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>VIN</t>
+          <t>K0</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>K0I</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>FOVI_1</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>K0</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>cbit0</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DRAIN_F</t>
+          <t>K1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R_DRAIN_A</t>
+          <t>VIN</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>K1</t>
+          <t>KVI</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>K0I</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>cbit1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DRAIN_S</t>
+          <t>K2</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R_DRAIN_A</t>
+          <t>K2I</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>K2</t>
+          <t>R_DRAIN_A</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>cbit2</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ROVP</t>
+          <t>K3</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>FOVI_3</t>
+          <t>K3I</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>K3</t>
+          <t>CL_A</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>FOVI_2_F</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>cbit3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CS_F</t>
+          <t>K4</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>FOVI_4_F</t>
+          <t>DRAIN_F</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>K4</t>
+          <t>K3I</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>K2I</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>cbit4</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CS_S</t>
+          <t>K5</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>FOVI_4_S</t>
+          <t>K5I</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>K5</t>
+          <t>R_DRAIN_A</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cbit2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DRAIN_F</t>
+          <t>K6</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>K6I</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CL_A</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>FOVI_2_F</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>K6</t>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>cbit3</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DRAIN_S</t>
+          <t>K7</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>FOVI_2_F</t>
+          <t>K7I</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>K7</t>
+          <t>FOVI_2_S</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>GND</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>cbit5</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>ROVP</t>
+          <t>K8</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R_ROVP_A</t>
+          <t>K8I</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>K8</t>
+          <t>K6I</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>K5I</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>cbit6</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>VIN</t>
+          <t>K9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KVI</t>
+          <t>DRAIN_S</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>K9</t>
+          <t>K7I</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>K8I</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>cbit7</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>DRAIN_F</t>
+          <t>K10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CL_A</t>
+          <t>K10I</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>K10</t>
+          <t>FOVI_3</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>cbit8</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>DRAIN_S</t>
+          <t>K11</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CL_A</t>
+          <t>ROVP</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>K11</t>
+          <t>R_ROVP_A</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>K10I</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>cbit9</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CS_F</t>
+          <t>K12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R_CS_A</t>
+          <t>K12I</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>K12</t>
+          <t>FOVI_4_F</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Float</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>cbit10</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CS_S</t>
+          <t>K13</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>CS_F</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>R_CS_A</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>K13</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>DRAIN_S</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>GND</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>K14</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>CS_S</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>GND</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>K15</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>DRAIN_S</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>FOVI_2_S</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>K16</t>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>K12I</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>cbit3</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>VCC</t>
         </is>
       </c>
     </row>

</xml_diff>